<commit_message>
Add CAMELSH resolution test files and analysis scripts
- Introduced new README.md for project documentation.
- Added configuration file (config.yaml) for setting parameters.
- Implemented inspect_camelsh.py notebook for dataset inspection.
- Created requirements.txt for package dependencies.
- Added run_operator_test.py script for operational testing.
- Initialized src directory with multiple Python modules for data handling:
  - aggregation.py
  - alignment.py
  - config.py
  - data_camels.py
  - data_usgs.py
  - metrics.py
- Updated event_metrics_vs_shifted_example_014.xlsx with new analysis results.
</commit_message>
<xml_diff>
--- a/Experiments/HPC_random_search/Analyze_HPC_results/event_metrics_vs_shifted_example_014.xlsx
+++ b/Experiments/HPC_random_search/Analyze_HPC_results/event_metrics_vs_shifted_example_014.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Python\neuralhydrology\Experiments\HPC_random_search\Analyze_HPC_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8824D7-50A4-4D63-A7CD-C2D3A8E579F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971C34D7-E50C-42DC-A4EF-B9E8340554B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,11 @@
     <sheet name="event_metrics" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1728,7 +1733,1153 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NSE -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> run_014</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="he-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>NSE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>event_metrics!$I$2:$I$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="107"/>
+                <c:pt idx="0">
+                  <c:v>0.86581071985331404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70171331241782897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27675768101174097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81145488189224502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55390056366669205</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46665050575700301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88254827066454899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.54595916875859E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.336216237219779</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48588981216231902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50076064742700399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.6831305419982801E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.40094789682460302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-9.7700939419825605E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8810898095679197E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.31266137449140202</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.0020370513790701E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.63455400755795</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.66164886675495005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.78704408463679798</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.6984936188303199E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.61275325811926296</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.61554010415553695</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.57207206624825602</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.112913429914863</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.47096601384043002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.18676135616160999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.59921876941667396</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.71296194101158405</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.890095394167982</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.86645710901676898</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.37116155629040498</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.74629099703186397</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.43056892804749403</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.49145617593146201</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.73671019420251505</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.49959006036874598</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.62788600797868199</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.75321182289391397</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.72721752046657495</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.230463318027742</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.39428781633945398</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.2267637648179102E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.159450627875978</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.70555598569730904</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.30680614887948698</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.84413323709772103</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47664939071113899</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.16338393720494099</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.65956333387931199</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.29127605489541503</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-0.47763093468733597</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.15369938026806401</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.71549294413540698</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.293316093043749</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.59964909729999705</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.52698505155125897</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.592711537004177</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.37524616898421698</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.71849431290855703</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.37338980431750302</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-0.29556287628678302</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.22638013049917599</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.93604492939345696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.87338013380907098</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.95021368211284596</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.62031152943365298</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.397407093470666</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.32813460677232098</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.78713816806311099</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.55363698231436898</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.29572426227770499</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.82105441355062703</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.42664759563932397</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.33171327959150698</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.687773779276173</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.26933055735371297</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.35188070957388801</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.57275907611126298</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.33869438133143298</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.55273383825046396</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.7357746962979802E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.20937542547381199</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.60297909169083497</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.53319222084199502</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.18550406133255801</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.27828681119046</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.56710076841023904</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.56721745051394201</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.66272549304322104</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.61575574051101001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.47228220936855397</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.60634741395764802</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.437048984765876</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.84973941072206205</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.28218691097515503</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.84935471139862195</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.46389202499027898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>event_metrics!$D$2:$D$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="107"/>
+                <c:pt idx="0">
+                  <c:v>0.86510185062174905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85336800875226104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44122343644850698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80766063291299095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63246321672664096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59068754517982602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91975724239932199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.187622700157735</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.9021795873920699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67456720837438799</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.46531067662980402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10879236744691</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27971896391170997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.162567397781433</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16810481387460699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.54078631263518095</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25651508735628298</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.81351768866767005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.78859954330784998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67796758185483696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.66613758224460595</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.64896304405768501</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.34107866901630501</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.55835553276722205</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.21952415045426599</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.223570932117483</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-34.810900035514898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.34719557663454098</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87338488020925797</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.91539407273487094</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.92822535895237801</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.60750187887847895</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.89675494752099305</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.41577803467322799</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.65132788008005804</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.82871462945756602</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.68116307619121896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.79413395505064799</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.89624557410302497</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.61069878445880299</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.2839397571901401</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.533902640317517</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.452054577600498</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.39519878547037102</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.80868502166633704</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.448303764158407</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.60026353446680103</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.382882130799722</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.59472080231365398</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.1818074281935599E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.257488305487862</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.88341552300460002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.26121556585053302</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.70109198439314602</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.59028158639206796</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.56804200282568995</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.72803623015139296</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.48697407858499703</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.6855655535461499E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.67204714196097504</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.36394015985286</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-4.0573737669333801E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.31482810182885501</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.95104096042708497</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.96722991450977303</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.98775841889935301</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.14340174213783999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.57126991823985596</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.45119614004523501</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.79465134184934805</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.63276185083846304</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.53169896649828396</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.80689513489334797</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.61772480246676098</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.49910167201105199</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.74523956085891196</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.62214268983536103</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.63690090347440598</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.65998510869079197</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.55512276365620306</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.69599466516567998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.25155684891848601</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.45505070610959802</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1.0978832768603</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.613282710197251</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.481134509654776</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.16815130103505799</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.62771449195849605</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.45672522779054198</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.36918918664252E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.83789609678719901</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.71377043094966997</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-0.38148475788118003</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.74735674716768496</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.69086749274902504</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.27947994914603902</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.94207326355522703</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.8817648829187398E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C9A5-443B-814E-81F7512E8097}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>01:01</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>event_metrics!$M$10:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>event_metrics!$N$10:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C9A5-443B-814E-81F7512E8097}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="818296575"/>
+        <c:axId val="818297823"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="818296575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Shifted</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> NSE</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="he-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818297823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="818297823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>NSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="he-IL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818296575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="he-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2284,6 +3435,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2317,6 +3984,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>103654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>350464</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52B9355-96F2-4DBE-BDB2-F500B6BB949D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2624,7 +4327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>

</xml_diff>